<commit_message>
Actualizacion de graficos y control de archivos
</commit_message>
<xml_diff>
--- a/tablaSismos.xlsx
+++ b/tablaSismos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\primerProyectoPOO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8845207E-AA48-4F0B-9401-0B470F674E08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D01C8CD-92FB-4A0A-84B5-8D015534A156}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,27 +115,6 @@
     <t>-83.1066</t>
   </si>
   <si>
-    <t>Mon Aug 20 22:58:39 CST 2018</t>
-  </si>
-  <si>
-    <t>Sat Aug 19 21:57:38 CST 2017</t>
-  </si>
-  <si>
-    <t>Sun Sep 09 11:47:28 CST 2007</t>
-  </si>
-  <si>
-    <t>Fri Jan 19 22:57:38 CST 2018</t>
-  </si>
-  <si>
-    <t>Tue Aug 14 16:52:33 CST 2012</t>
-  </si>
-  <si>
-    <t>Sat Apr 05 07:43:24 CST 2003</t>
-  </si>
-  <si>
-    <t>Tue Mar 05 07:43:24 CST 2018</t>
-  </si>
-  <si>
     <t>Detalle Falla</t>
   </si>
   <si>
@@ -169,42 +148,21 @@
     <t>Puntarenas</t>
   </si>
   <si>
-    <t>50 km al Suroeste de Jacó, Playa Hermosa de Garabito</t>
-  </si>
-  <si>
     <t>Lugar</t>
   </si>
   <si>
     <t>Terrestre</t>
   </si>
   <si>
-    <t>6.13 km hacia el Noreste de Puerto Armuelles, Panamá, Corredores de Puntarenas, Puerto Armuelles, Golfito, Puerto Jimenez, El Valle Central: Alajuela, Heredia, Escazú</t>
-  </si>
-  <si>
-    <t>3.68 km hacia el Noreste de Dos Rios de Osa de Puntarenas, Golfito, Puntarenas</t>
-  </si>
-  <si>
-    <t>3 km al SE de Paso Real, Buenos Aires, Puntarenas, Zona sur, Valle Central, Limón</t>
-  </si>
-  <si>
     <t>San_Jose</t>
   </si>
   <si>
-    <t>9.85 km al SO de las Juntas de Abangares, Las Juntas de Abangares, Nicoya, Santa Cruz, Nandayure, Cañas, Paquera, Miramar, Herradura Miramar, San Ramón, Palmares, Naranjo, Atenas, San Mateo, Turrucares.</t>
-  </si>
-  <si>
     <t>Guanacaste</t>
   </si>
   <si>
-    <t>Orosí, Cartago 3.9 Km SE, El Carmen y Tres Ríos, Cartago</t>
-  </si>
-  <si>
     <t>Cartago</t>
   </si>
   <si>
-    <t>Punta Banco, Golfito, Puntarenas, 2.6 Km de Bijagua de Upala, Fuerte en Punta Banco de Golfito, Puntarenas</t>
-  </si>
-  <si>
     <t>Marítimo</t>
   </si>
   <si>
@@ -212,6 +170,48 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>6.13 km hacia el Noreste de Puerto Armuelles</t>
+  </si>
+  <si>
+    <t>3.68 km hacia el Noreste de Dos Rios de Osa de Puntarenas</t>
+  </si>
+  <si>
+    <t>3 km al SE de Paso Real en Buenos Aires además Zona sur y  Valle Central</t>
+  </si>
+  <si>
+    <t>9.85 km al SO de las Juntas de Abangares en Nicoya y Santa Cruz.</t>
+  </si>
+  <si>
+    <t>Orosí 3.9 Km SE en El Carmen y Tres Ríos</t>
+  </si>
+  <si>
+    <t>Punta Banco en  Golfito 2.6 Km de Bijagua de Upala en Fuerte en Punta Banco de Golfito</t>
+  </si>
+  <si>
+    <t>50 km al Suroeste de Jacó en Playa Hermosa de Garabito</t>
+  </si>
+  <si>
+    <t>20-08-2020 22:58:39</t>
+  </si>
+  <si>
+    <t>19-08-2017 21:57:38</t>
+  </si>
+  <si>
+    <t>19-01-2018 22:57:38</t>
+  </si>
+  <si>
+    <t>09-09-2007 11:47:28</t>
+  </si>
+  <si>
+    <t>14-08-2012 16:52:33</t>
+  </si>
+  <si>
+    <t>05-04-2003 07:43:24</t>
+  </si>
+  <si>
+    <t>05-03-2018 07:43:24</t>
   </si>
 </sst>
 </file>
@@ -258,10 +258,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -586,7 +585,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +609,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -625,24 +624,24 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -654,27 +653,27 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -686,27 +685,27 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -718,141 +717,141 @@
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="4">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" s="5">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="4">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
         <v>35</v>
-      </c>
-      <c r="B6" s="5">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="5">
+        <v>62</v>
+      </c>
+      <c r="B7" s="4">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="5">
+        <v>63</v>
+      </c>
+      <c r="B8" s="4">
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="J8" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya se guardan los archivos en el Excel yupi!
</commit_message>
<xml_diff>
--- a/tablaSismos.xlsx
+++ b/tablaSismos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\primerProyectoPOO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C460B7B-BF77-4019-B46A-376C470E82DE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAFF51F-3FDF-40D0-B7F8-9723CE91A9D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2535" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -656,19 +656,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="28.5703125" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="10" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrección lectura de fecha gráfico en rango de fechas
</commit_message>
<xml_diff>
--- a/tablaSismos.xlsx
+++ b/tablaSismos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\primerProyectoPOO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAFF51F-3FDF-40D0-B7F8-9723CE91A9D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F842FD95-FFD2-4B86-BC17-51101CA7E2BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -656,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>

</xml_diff>